<commit_message>
sized all cells, awaiting layout
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Digital Design II\Proj1\repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Digital Design II\Proj1\repo\DD2P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -505,7 +505,7 @@
   <dimension ref="C2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,16 +546,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>16.502300000000002</v>
+        <v>30.676500000000001</v>
       </c>
       <c r="E5" s="2">
-        <v>29.061</v>
+        <v>42.613</v>
       </c>
       <c r="F5" s="2">
-        <v>50.898000000000003</v>
+        <v>62.825599999999902</v>
       </c>
       <c r="G5" s="3">
-        <v>88.305899999999994</v>
+        <v>99.671199999999999</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.3">
@@ -563,16 +563,16 @@
         <v>100</v>
       </c>
       <c r="D6" s="2">
-        <v>38.305</v>
+        <v>44.3431</v>
       </c>
       <c r="E6" s="2">
-        <v>50.071999999999903</v>
+        <v>54.093200000000003</v>
       </c>
       <c r="F6" s="2">
-        <v>69.087699999999998</v>
+        <v>70.593699999999998</v>
       </c>
       <c r="G6" s="3">
-        <v>104.485</v>
+        <v>104.97399999999899</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
@@ -580,16 +580,16 @@
         <v>400</v>
       </c>
       <c r="D7" s="2">
-        <v>59.893700000000003</v>
+        <v>64.761899999999997</v>
       </c>
       <c r="E7" s="2">
-        <v>79.944800000000001</v>
+        <v>79.717799999999997</v>
       </c>
       <c r="F7" s="2">
-        <v>112.413</v>
+        <v>105.06100000000001</v>
       </c>
       <c r="G7" s="3">
-        <v>163.40299999999999</v>
+        <v>147.202</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -597,16 +597,16 @@
         <v>800</v>
       </c>
       <c r="D8" s="4">
-        <v>75.2149</v>
+        <v>79.375299999999996</v>
       </c>
       <c r="E8" s="4">
-        <v>102.14100000000001</v>
+        <v>99.468299999999999</v>
       </c>
       <c r="F8" s="4">
-        <v>145.34700000000001</v>
+        <v>133.33199999999999</v>
       </c>
       <c r="G8" s="5">
-        <v>212.70400000000001</v>
+        <v>188.07300000000001</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -647,16 +647,16 @@
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <v>15.0344</v>
+        <v>28.814</v>
       </c>
       <c r="E12" s="2">
-        <v>27.023599999999998</v>
+        <v>33.734900000000003</v>
       </c>
       <c r="F12" s="2">
-        <v>41.106999999999999</v>
+        <v>43.6783</v>
       </c>
       <c r="G12" s="3">
-        <v>67.892600000000002</v>
+        <v>67.061400000000006</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.3">
@@ -664,16 +664,16 @@
         <v>100</v>
       </c>
       <c r="D13" s="2">
-        <v>38.866</v>
+        <v>44.037599999999998</v>
       </c>
       <c r="E13" s="2">
-        <v>49.562600000000003</v>
+        <v>51.9315</v>
       </c>
       <c r="F13" s="2">
-        <v>65.968500000000006</v>
+        <v>65.131100000000004</v>
       </c>
       <c r="G13" s="3">
-        <v>95.118600000000001</v>
+        <v>88.807699999999997</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.3">
@@ -681,16 +681,16 @@
         <v>400</v>
       </c>
       <c r="D14" s="2">
-        <v>69.465900000000005</v>
+        <v>75.836699999999993</v>
       </c>
       <c r="E14" s="2">
-        <v>89.732999999999905</v>
+        <v>90.438299999999998</v>
       </c>
       <c r="F14" s="2">
-        <v>121.09399999999999</v>
+        <v>114.505</v>
       </c>
       <c r="G14" s="3">
-        <v>168.38299999999899</v>
+        <v>153.483</v>
       </c>
     </row>
     <row r="15" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -698,16 +698,16 @@
         <v>800</v>
       </c>
       <c r="D15" s="4">
-        <v>94.531300000000002</v>
+        <v>102.681</v>
       </c>
       <c r="E15" s="4">
-        <v>122.179</v>
+        <v>122.295999999999</v>
       </c>
       <c r="F15" s="4">
-        <v>165.267</v>
+        <v>155.13300000000001</v>
       </c>
       <c r="G15" s="5">
-        <v>230.62</v>
+        <v>207.636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>